<commit_message>
Revise contract and invoice classes, add new features to the GUI, fix bugs, and update the to-do list.
</commit_message>
<xml_diff>
--- a/output/hung -  Resort.xlsx_output.xlsx
+++ b/output/hung -  Resort.xlsx_output.xlsx
@@ -175,112 +175,112 @@
     <t>, empty in Rate code, Date error in Arrival, Date error in Departure</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  TPL - JS  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-27  2023-09-01        75           -0.0           -0.0  ...        -0.0        -0.0              450.0       504.0       contract
-1 2023-09-02  2023-09-02        54           -0.0           -0.0  ...        -0.0        -0.0               54.0       504.0       contract
+    <t xml:space="preserve">  first date second date  TPL - JS  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-27  2023-09-01        75           -0.0  ...        -0.0              450.0        504.0       contract
+1 2023-09-02  2023-09-02        54           -0.0  ...        -0.0               54.0        504.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - DLX  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-22  2023-09-01         48           -0.0           -0.0  ...        -0.0        -0.0              528.0       560.0       contract
-1 2023-09-02  2023-09-02         32           -0.0           -0.0  ...        -0.0        -0.0               32.0       560.0       contract
+    <t xml:space="preserve">  first date second date  DBL - DLX  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-22  2023-09-01         48           -0.0  ...        -0.0              528.0        560.0       contract
+1 2023-09-02  2023-09-02         32           -0.0  ...        -0.0               32.0        560.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - DLX  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-27  2023-09-01         48           -0.0           -0.0  ...        -0.0        -0.0              288.0       320.0       contract
-1 2023-09-02  2023-09-02         32           -0.0           -0.0  ...        -0.0        -0.0               32.0       320.0       contract
+    <t xml:space="preserve">  first date second date  DBL - DLX  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-27  2023-09-01         48           -0.0  ...        -0.0              288.0        320.0       contract
+1 2023-09-02  2023-09-02         32           -0.0  ...        -0.0               32.0        320.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - STD  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-27  2023-09-01         42           -0.0           -0.0  ...        -0.0        -0.0              252.0       278.0       contract
-1 2023-09-02  2023-09-02         26           -0.0           -0.0  ...        -0.0        -0.0               26.0       278.0       contract
+    <t xml:space="preserve">  first date second date  DBL - STD  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-27  2023-09-01         42           -0.0  ...        -0.0              252.0        278.0       contract
+1 2023-09-02  2023-09-02         26           -0.0  ...        -0.0               26.0        278.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  SGL - JS  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-27  2023-09-01        37           -0.0           -0.0  ...        -0.0        -0.0              222.0       252.0       contract
-1 2023-09-02  2023-09-02        30           -0.0           -0.0  ...        -0.0        -0.0               30.0       252.0       contract
+    <t xml:space="preserve">  first date second date  SGL - JS  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-27  2023-09-01        37           -0.0  ...        -0.0              222.0        252.0       contract
+1 2023-09-02  2023-09-02        30           -0.0  ...        -0.0               30.0        252.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - JS   earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-27  2023-09-01         54           -0.0           -0.0  ...        -0.0        -0.0              324.0       364.0       contract
-1 2023-09-02  2023-09-02         40           -0.0           -0.0  ...        -0.0        -0.0               40.0       364.0       contract
+    <t xml:space="preserve">  first date second date  DBL - JS   earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-27  2023-09-01         54           -0.0  ...        -0.0              324.0        364.0       contract
+1 2023-09-02  2023-09-02         40           -0.0  ...        -0.0               40.0        364.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - DLX  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-24  2023-09-01         48           -0.0           -0.0  ...        -0.0        -0.0              432.0       464.0       contract
-1 2023-09-02  2023-09-02         32           -0.0           -0.0  ...        -0.0        -0.0               32.0       464.0       contract
+    <t xml:space="preserve">  first date second date  DBL - DLX  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-24  2023-09-01         48           -0.0  ...        -0.0              432.0        464.0       contract
+1 2023-09-02  2023-09-02         32           -0.0  ...        -0.0               32.0        464.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - STD  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-24  2023-09-01         42           -0.0           -0.0  ...        -0.0        -0.0              378.0       404.0       contract
-1 2023-09-02  2023-09-02         26           -0.0           -0.0  ...        -0.0        -0.0               26.0       404.0       contract
+    <t xml:space="preserve">  first date second date  DBL - STD  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-24  2023-09-01         42           -0.0  ...        -0.0              378.0        404.0       contract
+1 2023-09-02  2023-09-02         26           -0.0  ...        -0.0               26.0        404.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - DLX  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-09-03  2023-09-03         32           -0.0           -0.0  ...        -0.0        -0.0               32.0        32.0       contract
+    <t xml:space="preserve">  first date second date  DBL - DLX  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-09-03  2023-09-03         32           -0.0  ...        -0.0               32.0         32.0       contract
 [1 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  TPL - JS  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-09-03  2023-09-03        54           -0.0           -0.0  ...        -0.0        -0.0               54.0        54.0       contract
+    <t xml:space="preserve">  first date second date  TPL - JS  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-09-03  2023-09-03        54           -0.0  ...        -0.0               54.0         54.0       contract
 [1 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - JS   earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-09-03  2023-09-03         40           -0.0           -0.0  ...        -0.0        -0.0               40.0        40.0       contract
+    <t xml:space="preserve">  first date second date  DBL - JS   earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-09-03  2023-09-03         40           -0.0  ...        -0.0               40.0         40.0       contract
 [1 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - STD  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-09-03  2023-09-03         26           -0.0           -0.0  ...        -0.0        -0.0               26.0        26.0       contract
+    <t xml:space="preserve">  first date second date  DBL - STD  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-09-03  2023-09-03         26           -0.0  ...        -0.0               26.0         26.0       contract
 [1 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  SGL - JS  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-09-03  2023-09-03        30           -0.0           -0.0  ...        -0.0        -0.0               30.0        30.0       contract
+    <t xml:space="preserve">  first date second date  SGL - JS  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-09-03  2023-09-03        30           -0.0  ...        -0.0               30.0         30.0       contract
 [1 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - STD  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-30  2023-09-01         42           -0.0           -0.0  ...        -0.0        -0.0              126.0       230.0       contract
-1 2023-09-02  2023-09-05         26           -0.0           -0.0  ...        -0.0        -0.0              104.0       230.0       contract
+    <t xml:space="preserve">  first date second date  DBL - STD  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-30  2023-09-01         42           -0.0  ...        -0.0              126.0        230.0       contract
+1 2023-09-02  2023-09-05         26           -0.0  ...        -0.0              104.0        230.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - DLX  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-30  2023-09-01         48           -0.0           -0.0  ...        -0.0        -0.0              144.0       272.0       contract
-1 2023-09-02  2023-09-05         32           -0.0           -0.0  ...        -0.0        -0.0              128.0       272.0       contract
+    <t xml:space="preserve">  first date second date  DBL - DLX  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-30  2023-09-01         48           -0.0  ...        -0.0              144.0        272.0       contract
+1 2023-09-02  2023-09-05         32           -0.0  ...        -0.0              128.0        272.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  TPL - JS  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-30  2023-09-01        75           -0.0           -0.0  ...        -0.0        -0.0              225.0       441.0       contract
-1 2023-09-02  2023-09-05        54           -0.0           -0.0  ...        -0.0        -0.0              216.0       441.0       contract
+    <t xml:space="preserve">  first date second date  TPL - JS  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-30  2023-09-01        75           -0.0  ...        -0.0              225.0        441.0       contract
+1 2023-09-02  2023-09-05        54           -0.0  ...        -0.0              216.0        441.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - JS   earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-30  2023-09-01         54           -0.0           -0.0  ...        -0.0        -0.0              162.0       322.0       contract
-1 2023-09-02  2023-09-05         40           -0.0           -0.0  ...        -0.0        -0.0              160.0       322.0       contract
+    <t xml:space="preserve">  first date second date  DBL - JS   earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-30  2023-09-01         54           -0.0  ...        -0.0              162.0        322.0       contract
+1 2023-09-02  2023-09-05         40           -0.0  ...        -0.0              160.0        322.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  SGL - DLX  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-30  2023-09-01         34           -0.0           -0.0  ...        -0.0        -0.0              102.0       206.0       contract
-1 2023-09-02  2023-09-05         26           -0.0           -0.0  ...        -0.0        -0.0              104.0       206.0       contract
+    <t xml:space="preserve">  first date second date  SGL - DLX  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-30  2023-09-01         34           -0.0  ...        -0.0              102.0        206.0       contract
+1 2023-09-02  2023-09-05         26           -0.0  ...        -0.0              104.0        206.0       contract
 [2 rows x 15 columns]</t>
   </si>
   <si>
-    <t xml:space="preserve">  first date second date  DBL - DLX  earlyBooking1  earlyBooking2  ...  Reduction1  Reduction2  price with offers total price  contract name
-0 2023-08-24  2023-09-01         48           -0.0           -0.0  ...        -0.0        -0.0              432.0       560.0       contract
-1 2023-09-02  2023-09-05         32           -0.0           -0.0  ...        -0.0        -0.0              128.0       560.0       contract
+    <t xml:space="preserve">  first date second date  DBL - DLX  earlyBooking1  ...  Reduction2  price with offers  total price  contract name
+0 2023-08-24  2023-09-01         48           -0.0  ...        -0.0              432.0        560.0       contract
+1 2023-09-02  2023-09-05         32           -0.0  ...        -0.0              128.0        560.0       contract
 [2 rows x 15 columns]</t>
   </si>
 </sst>

</xml_diff>